<commit_message>
update change TinhLai -> loi nhuan
</commit_message>
<xml_diff>
--- a/TailieuDA/DA_QLcuahangmaytinh.xlsx
+++ b/TailieuDA/DA_QLcuahangmaytinh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BT_FREELANCE\QLKhoMayTinh\TailieuDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BT_FREELANCE\QLKho\TailieuDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC1395B-2EE4-4316-A3B6-7F1F1798DC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF722F3-B08F-48C1-9905-378BAAC5CBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6876" yWindow="4044" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Các thành phần cần thay đổi" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>stt</t>
   </si>
@@ -138,9 +138,6 @@
     <t xml:space="preserve">thay đổi giao diện theo hướng phân quyền. Admin sẽ quản lý User(chấm công, quản lý giờ giấc), User sẽ quản lý sản phẩm (quản lý đặt hàng, xuất hàng, quản lý các nhà cung cấp). </t>
   </si>
   <si>
-    <t>Giang</t>
-  </si>
-  <si>
     <t>Ghi chú</t>
   </si>
   <si>
@@ -156,18 +153,9 @@
     <t>các sơ đồ thiết kế hệ thống, update giao diện phân quyền admin-user</t>
   </si>
   <si>
-    <t>1tr</t>
-  </si>
-  <si>
     <t>thêm option, tính lãi</t>
   </si>
   <si>
-    <t>3tr</t>
-  </si>
-  <si>
-    <t>Dinh</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -178,17 +166,30 @@
   </si>
   <si>
     <t>26/11/2024</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -301,55 +302,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -358,12 +359,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +584,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -622,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -666,7 +668,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -686,10 +688,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,7 +706,7 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -720,8 +722,8 @@
       <c r="D7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>33</v>
+      <c r="E7" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -735,26 +737,26 @@
     <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -762,21 +764,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>39</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D18" s="24"/>
     </row>
     <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>2</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="22">
         <v>45363</v>
@@ -788,16 +788,14 @@
         <v>3</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C20" s="22">
         <v>45577</v>
       </c>
-      <c r="D20" s="24" t="s">
-        <v>41</v>
-      </c>
+      <c r="D20" s="24"/>
       <c r="I20" s="14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update loi nhuan, nha cung cap
</commit_message>
<xml_diff>
--- a/TailieuDA/DA_QLcuahangmaytinh.xlsx
+++ b/TailieuDA/DA_QLcuahangmaytinh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BT_FREELANCE\QLKho\TailieuDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF722F3-B08F-48C1-9905-378BAAC5CBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6533755-06F0-4671-A242-58D485740BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6876" yWindow="4044" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>thiết lập công thức tính công cho nhân viên</t>
   </si>
   <si>
-    <t>tính lãi</t>
-  </si>
-  <si>
     <t>căn cứ vào từng mặt hàng mà lãi sản phẩm cố định ở theo từng mức 5%, 10%, 20%</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>lợi nhuận</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -668,7 +668,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -682,16 +682,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -699,14 +699,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -714,16 +714,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -737,26 +737,26 @@
     <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,10 +764,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="24"/>
     </row>
@@ -776,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="22">
         <v>45363</v>
@@ -788,14 +788,14 @@
         <v>3</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="22">
         <v>45577</v>
       </c>
       <c r="D20" s="24"/>
       <c r="I20" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -1837,7 +1837,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1845,10 +1845,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="9">
@@ -1861,10 +1861,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="9">
@@ -1880,7 +1880,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="9">
@@ -1893,10 +1893,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="9">
@@ -1909,10 +1909,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="9">
@@ -1925,10 +1925,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="9">

</xml_diff>